<commit_message>
Update to Reference Doc
</commit_message>
<xml_diff>
--- a/Ref Docs/Font Size for Different Scales.xlsx
+++ b/Ref Docs/Font Size for Different Scales.xlsx
@@ -87,7 +87,7 @@
     <t>Enter Info below</t>
   </si>
   <si>
-    <t>Below is the font size at various scales. Entere additional scales as needed</t>
+    <t>Below is the font size at various scales. Enter additional scales as needed</t>
   </si>
 </sst>
 </file>
@@ -95,7 +95,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.0000"/>
+    <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -333,6 +333,58 @@
   </cellStyleXfs>
   <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -345,69 +397,17 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -750,416 +750,416 @@
   <dimension ref="B1:N39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3:F3"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3" style="8" customWidth="1"/>
-    <col min="2" max="2" width="43.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.42578125" style="7" customWidth="1"/>
-    <col min="6" max="6" width="19.140625" style="9" customWidth="1"/>
-    <col min="7" max="7" width="9.140625" style="8"/>
-    <col min="8" max="8" width="43.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6" style="8" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.140625" style="8"/>
-    <col min="11" max="11" width="12.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12" style="8" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.140625" style="8"/>
-    <col min="14" max="14" width="43.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="15" max="16384" width="9.140625" style="8"/>
+    <col min="1" max="1" width="3" style="4" customWidth="1"/>
+    <col min="2" max="2" width="43.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.42578125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="19.140625" style="5" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" style="4"/>
+    <col min="8" max="8" width="43.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.140625" style="4"/>
+    <col min="11" max="11" width="12.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12" style="4" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.140625" style="4"/>
+    <col min="14" max="14" width="43.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="2"/>
+      <c r="C2" s="20"/>
     </row>
     <row r="3" spans="2:14" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="4"/>
-      <c r="E3" s="20" t="s">
+      <c r="C3" s="22"/>
+      <c r="E3" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="19"/>
+      <c r="F3" s="26"/>
     </row>
     <row r="4" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
     </row>
     <row r="5" spans="2:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="25" t="s">
+      <c r="B5" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="26"/>
-      <c r="E5" s="23" t="s">
+      <c r="C5" s="24"/>
+      <c r="E5" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="F5" s="24" t="s">
+      <c r="F5" s="18" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B6" s="17" t="s">
+      <c r="B6" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="18">
+      <c r="C6" s="14">
         <v>720</v>
       </c>
-      <c r="E6" s="21">
+      <c r="E6" s="15">
         <v>60</v>
       </c>
-      <c r="F6" s="22">
+      <c r="F6" s="16">
         <f>($C$7/$C$6)*E6</f>
         <v>0.52083333333333337</v>
       </c>
     </row>
     <row r="7" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="15" t="s">
+      <c r="B7" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="16">
+      <c r="C7" s="12">
         <v>6.25</v>
       </c>
-      <c r="E7" s="10">
+      <c r="E7" s="6">
         <f>E6+60</f>
         <v>120</v>
       </c>
-      <c r="F7" s="11">
+      <c r="F7" s="7">
         <f t="shared" ref="F7:F39" si="0">($C$7/$C$6)*E7</f>
         <v>1.0416666666666667</v>
       </c>
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B8" s="6"/>
-      <c r="E8" s="10">
+      <c r="B8" s="2"/>
+      <c r="E8" s="6">
         <f t="shared" ref="E8:E39" si="1">E7+60</f>
         <v>180</v>
       </c>
-      <c r="F8" s="11">
+      <c r="F8" s="7">
         <f t="shared" si="0"/>
         <v>1.5625</v>
       </c>
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="E9" s="10">
+      <c r="E9" s="6">
         <f t="shared" si="1"/>
         <v>240</v>
       </c>
-      <c r="F9" s="11">
+      <c r="F9" s="7">
         <f t="shared" si="0"/>
         <v>2.0833333333333335</v>
       </c>
-      <c r="H9" s="12"/>
-      <c r="N9" s="12"/>
+      <c r="H9" s="8"/>
+      <c r="N9" s="8"/>
     </row>
     <row r="10" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="E10" s="10">
+      <c r="E10" s="6">
         <f t="shared" si="1"/>
         <v>300</v>
       </c>
-      <c r="F10" s="11">
+      <c r="F10" s="7">
         <f t="shared" si="0"/>
         <v>2.604166666666667</v>
       </c>
-      <c r="H10" s="13"/>
-      <c r="N10" s="13"/>
+      <c r="H10" s="9"/>
+      <c r="N10" s="9"/>
     </row>
     <row r="11" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="E11" s="10">
+      <c r="E11" s="6">
         <f t="shared" si="1"/>
         <v>360</v>
       </c>
-      <c r="F11" s="11">
+      <c r="F11" s="7">
         <f t="shared" si="0"/>
         <v>3.125</v>
       </c>
     </row>
     <row r="12" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="E12" s="10">
+      <c r="E12" s="6">
         <f t="shared" si="1"/>
         <v>420</v>
       </c>
-      <c r="F12" s="11">
+      <c r="F12" s="7">
         <f t="shared" si="0"/>
         <v>3.6458333333333335</v>
       </c>
     </row>
     <row r="13" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="E13" s="10">
+      <c r="E13" s="6">
         <f t="shared" si="1"/>
         <v>480</v>
       </c>
-      <c r="F13" s="11">
+      <c r="F13" s="7">
         <f t="shared" si="0"/>
         <v>4.166666666666667</v>
       </c>
     </row>
     <row r="14" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B14" s="8" t="s">
+      <c r="B14" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E14" s="10">
+      <c r="E14" s="6">
         <f t="shared" si="1"/>
         <v>540</v>
       </c>
-      <c r="F14" s="11">
+      <c r="F14" s="7">
         <f t="shared" si="0"/>
         <v>4.6875</v>
       </c>
     </row>
     <row r="15" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="E15" s="10">
+      <c r="E15" s="6">
         <f t="shared" si="1"/>
         <v>600</v>
       </c>
-      <c r="F15" s="11">
+      <c r="F15" s="7">
         <f t="shared" si="0"/>
         <v>5.2083333333333339</v>
       </c>
     </row>
     <row r="16" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="E16" s="10">
+      <c r="E16" s="6">
         <f t="shared" si="1"/>
         <v>660</v>
       </c>
-      <c r="F16" s="11">
+      <c r="F16" s="7">
         <f t="shared" si="0"/>
         <v>5.729166666666667</v>
       </c>
     </row>
     <row r="17" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E17" s="10">
+      <c r="E17" s="6">
         <f t="shared" si="1"/>
         <v>720</v>
       </c>
-      <c r="F17" s="11">
+      <c r="F17" s="7">
         <f t="shared" si="0"/>
         <v>6.25</v>
       </c>
     </row>
     <row r="18" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E18" s="10">
+      <c r="E18" s="6">
         <f t="shared" si="1"/>
         <v>780</v>
       </c>
-      <c r="F18" s="11">
+      <c r="F18" s="7">
         <f t="shared" si="0"/>
         <v>6.7708333333333339</v>
       </c>
     </row>
     <row r="19" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E19" s="10">
+      <c r="E19" s="6">
         <f t="shared" si="1"/>
         <v>840</v>
       </c>
-      <c r="F19" s="11">
+      <c r="F19" s="7">
         <f t="shared" si="0"/>
         <v>7.291666666666667</v>
       </c>
     </row>
     <row r="20" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E20" s="10">
+      <c r="E20" s="6">
         <f t="shared" si="1"/>
         <v>900</v>
       </c>
-      <c r="F20" s="11">
+      <c r="F20" s="7">
         <f t="shared" si="0"/>
         <v>7.8125</v>
       </c>
     </row>
     <row r="21" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E21" s="10">
+      <c r="E21" s="6">
         <f t="shared" si="1"/>
         <v>960</v>
       </c>
-      <c r="F21" s="11">
+      <c r="F21" s="7">
         <f t="shared" si="0"/>
         <v>8.3333333333333339</v>
       </c>
     </row>
     <row r="22" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E22" s="10">
+      <c r="E22" s="6">
         <f t="shared" si="1"/>
         <v>1020</v>
       </c>
-      <c r="F22" s="11">
+      <c r="F22" s="7">
         <f t="shared" si="0"/>
         <v>8.8541666666666679</v>
       </c>
     </row>
     <row r="23" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E23" s="10">
+      <c r="E23" s="6">
         <f t="shared" si="1"/>
         <v>1080</v>
       </c>
-      <c r="F23" s="11">
+      <c r="F23" s="7">
         <f t="shared" si="0"/>
         <v>9.375</v>
       </c>
     </row>
     <row r="24" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E24" s="10">
+      <c r="E24" s="6">
         <f t="shared" si="1"/>
         <v>1140</v>
       </c>
-      <c r="F24" s="11">
+      <c r="F24" s="7">
         <f t="shared" si="0"/>
         <v>9.8958333333333339</v>
       </c>
     </row>
     <row r="25" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E25" s="10">
+      <c r="E25" s="6">
         <f t="shared" si="1"/>
         <v>1200</v>
       </c>
-      <c r="F25" s="11">
+      <c r="F25" s="7">
         <f t="shared" si="0"/>
         <v>10.416666666666668</v>
       </c>
     </row>
     <row r="26" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E26" s="10">
+      <c r="E26" s="6">
         <f t="shared" si="1"/>
         <v>1260</v>
       </c>
-      <c r="F26" s="11">
+      <c r="F26" s="7">
         <f t="shared" si="0"/>
         <v>10.9375</v>
       </c>
     </row>
     <row r="27" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E27" s="10">
+      <c r="E27" s="6">
         <f t="shared" si="1"/>
         <v>1320</v>
       </c>
-      <c r="F27" s="11">
+      <c r="F27" s="7">
         <f t="shared" si="0"/>
         <v>11.458333333333334</v>
       </c>
     </row>
     <row r="28" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E28" s="10">
+      <c r="E28" s="6">
         <f t="shared" si="1"/>
         <v>1380</v>
       </c>
-      <c r="F28" s="11">
+      <c r="F28" s="7">
         <f t="shared" si="0"/>
         <v>11.979166666666668</v>
       </c>
     </row>
     <row r="29" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E29" s="10">
+      <c r="E29" s="6">
         <f t="shared" si="1"/>
         <v>1440</v>
       </c>
-      <c r="F29" s="11">
+      <c r="F29" s="7">
         <f t="shared" si="0"/>
         <v>12.5</v>
       </c>
     </row>
     <row r="30" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E30" s="10">
+      <c r="E30" s="6">
         <f t="shared" si="1"/>
         <v>1500</v>
       </c>
-      <c r="F30" s="11">
+      <c r="F30" s="7">
         <f t="shared" si="0"/>
         <v>13.020833333333334</v>
       </c>
     </row>
     <row r="31" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E31" s="10">
+      <c r="E31" s="6">
         <f t="shared" si="1"/>
         <v>1560</v>
       </c>
-      <c r="F31" s="11">
+      <c r="F31" s="7">
         <f t="shared" si="0"/>
         <v>13.541666666666668</v>
       </c>
     </row>
     <row r="32" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E32" s="10">
+      <c r="E32" s="6">
         <f t="shared" si="1"/>
         <v>1620</v>
       </c>
-      <c r="F32" s="11">
+      <c r="F32" s="7">
         <f t="shared" si="0"/>
         <v>14.0625</v>
       </c>
     </row>
     <row r="33" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E33" s="10">
+      <c r="E33" s="6">
         <f t="shared" si="1"/>
         <v>1680</v>
       </c>
-      <c r="F33" s="11">
+      <c r="F33" s="7">
         <f t="shared" si="0"/>
         <v>14.583333333333334</v>
       </c>
     </row>
     <row r="34" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E34" s="10">
+      <c r="E34" s="6">
         <f t="shared" si="1"/>
         <v>1740</v>
       </c>
-      <c r="F34" s="11">
+      <c r="F34" s="7">
         <f t="shared" si="0"/>
         <v>15.104166666666668</v>
       </c>
     </row>
     <row r="35" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E35" s="10">
+      <c r="E35" s="6">
         <f t="shared" si="1"/>
         <v>1800</v>
       </c>
-      <c r="F35" s="11">
+      <c r="F35" s="7">
         <f t="shared" si="0"/>
         <v>15.625</v>
       </c>
     </row>
     <row r="36" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E36" s="10">
+      <c r="E36" s="6">
         <f t="shared" si="1"/>
         <v>1860</v>
       </c>
-      <c r="F36" s="11">
+      <c r="F36" s="7">
         <f t="shared" si="0"/>
         <v>16.145833333333336</v>
       </c>
     </row>
     <row r="37" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E37" s="10">
+      <c r="E37" s="6">
         <f t="shared" si="1"/>
         <v>1920</v>
       </c>
-      <c r="F37" s="11">
+      <c r="F37" s="7">
         <f t="shared" si="0"/>
         <v>16.666666666666668</v>
       </c>
     </row>
     <row r="38" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E38" s="10">
+      <c r="E38" s="6">
         <f t="shared" si="1"/>
         <v>1980</v>
       </c>
-      <c r="F38" s="11">
+      <c r="F38" s="7">
         <f t="shared" si="0"/>
         <v>17.1875</v>
       </c>
     </row>
     <row r="39" spans="5:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E39" s="14">
+      <c r="E39" s="10">
         <f t="shared" si="1"/>
         <v>2040</v>
       </c>
-      <c r="F39" s="11">
+      <c r="F39" s="7">
         <f t="shared" si="0"/>
         <v>17.708333333333336</v>
       </c>

</xml_diff>